<commit_message>
SOLVED versions of activity spreadsheets.
</commit_message>
<xml_diff>
--- a/Classes/2021-04-26/01-GradeBook_Unsolved.xlsx
+++ b/Classes/2021-04-26/01-GradeBook_Unsolved.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrm\Desktop\CodeNew\_Analytics-GitHub\Classes\2021-04-26\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87878FF9-7CC1-4098-9D09-0EABE693AA5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C793BB9-8795-49C1-B7F2-FD7B92455A1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5590" yWindow="340" windowWidth="12980" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Student Name</t>
   </si>
@@ -121,9 +130,6 @@
   </si>
   <si>
     <t>Pass/Fail</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -503,7 +509,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -555,8 +561,17 @@
       <c r="E2" s="2">
         <v>56</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>32</v>
+      <c r="F2" s="2">
+        <f>ROUND(AVERAGE(B2:E2),0)</f>
+        <v>79</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(F2&gt;60,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(F2&gt;=90,"A",IF(F2&gt;=80,"B",IF(F2&gt;=70,"C",IF(F2&gt;=60,"D","F"))))</f>
+        <v>C</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -575,7 +590,18 @@
       <c r="E3" s="2">
         <v>95</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F25" si="0">ROUND(AVERAGE(B3:E3),0)</f>
+        <v>74</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G25" si="1">IF(F3&gt;60,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H25" si="2">IF(F3&gt;=90,"A",IF(F3&gt;=80,"B",IF(F3&gt;=70,"C",IF(F3&gt;=60,"D","F"))))</f>
+        <v>C</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -593,7 +619,18 @@
       <c r="E4" s="2">
         <v>87</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -611,7 +648,18 @@
       <c r="E5" s="2">
         <v>63</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>FAIL</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -629,7 +677,18 @@
       <c r="E6" s="2">
         <v>85</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v>B</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -647,7 +706,18 @@
       <c r="E7" s="2">
         <v>55</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="2"/>
+        <v>C</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -665,7 +735,18 @@
       <c r="E8" s="2">
         <v>83</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v>B</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -683,7 +764,18 @@
       <c r="E9" s="2">
         <v>43</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>FAIL</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -701,7 +793,18 @@
       <c r="E10" s="2">
         <v>95</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -719,7 +822,18 @@
       <c r="E11" s="2">
         <v>47</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>FAIL</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>D</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -737,7 +851,18 @@
       <c r="E12" s="2">
         <v>55</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>FAIL</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -755,7 +880,18 @@
       <c r="E13" s="2">
         <v>46</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>FAIL</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>D</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -773,7 +909,18 @@
       <c r="E14" s="2">
         <v>52</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>FAIL</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -791,7 +938,18 @@
       <c r="E15" s="2">
         <v>57</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="2"/>
+        <v>D</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -809,9 +967,20 @@
       <c r="E16" s="2">
         <v>73</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -827,9 +996,20 @@
       <c r="E17" s="2">
         <v>53</v>
       </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -845,9 +1025,20 @@
       <c r="E18" s="2">
         <v>97</v>
       </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -863,9 +1054,20 @@
       <c r="E19" s="2">
         <v>89</v>
       </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="2">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -881,9 +1083,20 @@
       <c r="E20" s="2">
         <v>82</v>
       </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F20" s="2">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -899,9 +1112,20 @@
       <c r="E21" s="2">
         <v>87</v>
       </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F21" s="2">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -917,9 +1141,20 @@
       <c r="E22" s="2">
         <v>100</v>
       </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F22" s="2">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -935,9 +1170,20 @@
       <c r="E23" s="2">
         <v>48</v>
       </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F23" s="2">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>FAIL</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -953,9 +1199,20 @@
       <c r="E24" s="2">
         <v>55</v>
       </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F24" s="2">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>FAIL</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -971,7 +1228,18 @@
       <c r="E25" s="2">
         <v>53</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="2">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>D</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>